<commit_message>
Current planning Tiling textures
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="643">
   <si>
     <t>Arne</t>
   </si>
@@ -10312,8 +10312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="J16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11156,7 +11156,7 @@
         <v>152</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>336</v>
+        <v>253</v>
       </c>
       <c r="M35" s="23"/>
       <c r="N35" s="8" t="s">
@@ -11175,6 +11175,9 @@
       <c r="S35" s="14"/>
       <c r="T35" s="8" t="s">
         <v>254</v>
+      </c>
+      <c r="U35" s="8" t="s">
+        <v>336</v>
       </c>
       <c r="V35" s="14"/>
       <c r="Y35" s="14"/>
@@ -11206,7 +11209,7 @@
         <v>154</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>337</v>
+        <v>256</v>
       </c>
       <c r="M36" s="23"/>
       <c r="N36" s="8" t="s">
@@ -11225,6 +11228,9 @@
       <c r="S36" s="14"/>
       <c r="T36" s="8" t="s">
         <v>264</v>
+      </c>
+      <c r="U36" s="8" t="s">
+        <v>337</v>
       </c>
       <c r="V36" s="14"/>
       <c r="Y36" s="14"/>
@@ -11256,7 +11262,7 @@
         <v>504</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>339</v>
+        <v>266</v>
       </c>
       <c r="M37" s="23"/>
       <c r="N37" s="8" t="s">
@@ -11275,6 +11281,9 @@
       <c r="S37" s="14"/>
       <c r="T37" s="8" t="s">
         <v>475</v>
+      </c>
+      <c r="U37" s="8" t="s">
+        <v>339</v>
       </c>
       <c r="V37" s="14"/>
       <c r="Y37" s="14"/>
@@ -11306,7 +11315,7 @@
         <v>570</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>344</v>
+        <v>254</v>
       </c>
       <c r="M38" s="23"/>
       <c r="N38" s="8" t="s">
@@ -11325,6 +11334,9 @@
       <c r="S38" s="14"/>
       <c r="T38" s="8" t="s">
         <v>608</v>
+      </c>
+      <c r="U38" s="8" t="s">
+        <v>344</v>
       </c>
       <c r="V38" s="14"/>
       <c r="Y38" s="14"/>
@@ -11345,12 +11357,15 @@
         <v>574</v>
       </c>
       <c r="G39" s="14"/>
+      <c r="I39" s="8" t="s">
+        <v>504</v>
+      </c>
       <c r="J39" s="14"/>
       <c r="K39" s="8" t="s">
         <v>506</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>345</v>
+        <v>264</v>
       </c>
       <c r="M39" s="23"/>
       <c r="N39" s="8" t="s">
@@ -11367,6 +11382,12 @@
         <v>291</v>
       </c>
       <c r="S39" s="14"/>
+      <c r="T39" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="U39" s="8" t="s">
+        <v>345</v>
+      </c>
       <c r="V39" s="14"/>
       <c r="Y39" s="14"/>
     </row>
@@ -11380,13 +11401,13 @@
       </c>
       <c r="D40" s="14"/>
       <c r="G40" s="14"/>
+      <c r="I40" s="5" t="s">
+        <v>570</v>
+      </c>
       <c r="J40" s="14"/>
       <c r="K40" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="L40" s="8" t="s">
-        <v>350</v>
-      </c>
       <c r="M40" s="23"/>
       <c r="N40" s="8" t="s">
         <v>164</v>
@@ -11399,6 +11420,12 @@
         <v>293</v>
       </c>
       <c r="S40" s="14"/>
+      <c r="T40" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="U40" s="8" t="s">
+        <v>350</v>
+      </c>
       <c r="V40" s="14"/>
       <c r="Y40" s="14"/>
     </row>
@@ -11412,13 +11439,13 @@
       </c>
       <c r="D41" s="14"/>
       <c r="G41" s="14"/>
+      <c r="I41" s="8" t="s">
+        <v>506</v>
+      </c>
       <c r="J41" s="14"/>
       <c r="K41" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="L41" s="8" t="s">
-        <v>351</v>
-      </c>
       <c r="M41" s="23"/>
       <c r="N41" s="8" t="s">
         <v>237</v>
@@ -11431,6 +11458,12 @@
         <v>258</v>
       </c>
       <c r="S41" s="14"/>
+      <c r="T41" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="U41" s="8" t="s">
+        <v>351</v>
+      </c>
       <c r="V41" s="14"/>
       <c r="Y41" s="14"/>
     </row>
@@ -11444,13 +11477,13 @@
       </c>
       <c r="D42" s="14"/>
       <c r="G42" s="14"/>
+      <c r="I42" s="8" t="s">
+        <v>376</v>
+      </c>
       <c r="J42" s="14"/>
       <c r="K42" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="L42" s="8" t="s">
-        <v>356</v>
-      </c>
       <c r="M42" s="23"/>
       <c r="N42" s="8" t="s">
         <v>238</v>
@@ -11463,6 +11496,12 @@
         <v>259</v>
       </c>
       <c r="S42" s="14"/>
+      <c r="T42" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="U42" s="8" t="s">
+        <v>356</v>
+      </c>
       <c r="V42" s="14"/>
       <c r="Y42" s="14"/>
     </row>
@@ -11476,10 +11515,10 @@
       </c>
       <c r="D43" s="22"/>
       <c r="G43" s="14"/>
+      <c r="I43" s="8" t="s">
+        <v>377</v>
+      </c>
       <c r="J43" s="14"/>
-      <c r="L43" s="8" t="s">
-        <v>355</v>
-      </c>
       <c r="M43" s="23"/>
       <c r="N43" s="8" t="s">
         <v>239</v>
@@ -11489,6 +11528,12 @@
         <v>260</v>
       </c>
       <c r="S43" s="14"/>
+      <c r="T43" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="U43" s="8" t="s">
+        <v>355</v>
+      </c>
       <c r="V43" s="14"/>
       <c r="Y43" s="14"/>
     </row>
@@ -11500,10 +11545,16 @@
       <c r="C44" s="21"/>
       <c r="D44" s="22"/>
       <c r="G44" s="14"/>
+      <c r="I44" s="8" t="s">
+        <v>375</v>
+      </c>
       <c r="J44" s="14"/>
       <c r="M44" s="23"/>
       <c r="P44" s="14"/>
       <c r="S44" s="14"/>
+      <c r="T44" s="8" t="s">
+        <v>375</v>
+      </c>
       <c r="V44" s="14"/>
       <c r="Y44" s="14"/>
     </row>

</xml_diff>

<commit_message>
Mijn assest in mijn scene gezet en de planning bijgewerkt
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enra\Documents\KappaSquad\Concept\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliek\OneDrive\Documenten\KappaSquad\Concept\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2221" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2215" uniqueCount="643">
   <si>
     <t>Arne</t>
   </si>
@@ -4434,8 +4434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J363"/>
   <sheetViews>
-    <sheetView topLeftCell="B297" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C307" sqref="C307:C310"/>
+    <sheetView topLeftCell="B27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10312,8 +10312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R41" sqref="R41"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10603,12 +10603,15 @@
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="I11" s="20" t="s">
         <v>529</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="J11" s="14"/>
+      <c r="K11" s="20" t="s">
         <v>387</v>
       </c>
-      <c r="J11" s="14"/>
       <c r="M11" s="23"/>
       <c r="P11" s="14"/>
       <c r="S11" s="14"/>
@@ -10623,9 +10626,6 @@
       <c r="D12" s="14"/>
       <c r="E12" s="20" t="s">
         <v>393</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>394</v>
       </c>
       <c r="G12" s="14"/>
       <c r="J12" s="14"/>
@@ -10962,15 +10962,12 @@
         <v>527</v>
       </c>
       <c r="D28" s="14"/>
-      <c r="E28" s="20" t="s">
-        <v>188</v>
-      </c>
       <c r="G28" s="14"/>
       <c r="H28" s="20" t="s">
-        <v>229</v>
+        <v>633</v>
       </c>
       <c r="I28" s="20" t="s">
-        <v>189</v>
+        <v>634</v>
       </c>
       <c r="J28" s="14"/>
       <c r="K28" s="20" t="s">
@@ -10988,10 +10985,10 @@
       </c>
       <c r="P28" s="14"/>
       <c r="Q28" s="20" t="s">
-        <v>633</v>
+        <v>188</v>
       </c>
       <c r="R28" s="20" t="s">
-        <v>634</v>
+        <v>189</v>
       </c>
       <c r="S28" s="14"/>
       <c r="T28" s="20" t="s">
@@ -11019,6 +11016,9 @@
       <c r="J29" s="14"/>
       <c r="M29" s="23"/>
       <c r="P29" s="14"/>
+      <c r="R29" s="20" t="s">
+        <v>229</v>
+      </c>
       <c r="S29" s="14"/>
       <c r="V29" s="14"/>
       <c r="W29" s="20" t="s">
@@ -11279,9 +11279,6 @@
         <v>293</v>
       </c>
       <c r="S37" s="14"/>
-      <c r="T37" s="8" t="s">
-        <v>504</v>
-      </c>
       <c r="U37" s="8" t="s">
         <v>339</v>
       </c>
@@ -11311,7 +11308,7 @@
         <v>357</v>
       </c>
       <c r="J38" s="14"/>
-      <c r="K38" s="5" t="s">
+      <c r="K38" s="8" t="s">
         <v>570</v>
       </c>
       <c r="L38" s="8" t="s">
@@ -11332,9 +11329,6 @@
         <v>258</v>
       </c>
       <c r="S38" s="14"/>
-      <c r="T38" s="5" t="s">
-        <v>570</v>
-      </c>
       <c r="U38" s="8" t="s">
         <v>344</v>
       </c>
@@ -11382,9 +11376,6 @@
         <v>259</v>
       </c>
       <c r="S39" s="14"/>
-      <c r="T39" s="8" t="s">
-        <v>506</v>
-      </c>
       <c r="U39" s="8" t="s">
         <v>345</v>
       </c>
@@ -11401,7 +11392,7 @@
       </c>
       <c r="D40" s="14"/>
       <c r="G40" s="14"/>
-      <c r="I40" s="5" t="s">
+      <c r="I40" s="8" t="s">
         <v>570</v>
       </c>
       <c r="J40" s="14"/>
@@ -11420,9 +11411,6 @@
         <v>260</v>
       </c>
       <c r="S40" s="14"/>
-      <c r="T40" s="8" t="s">
-        <v>376</v>
-      </c>
       <c r="U40" s="8" t="s">
         <v>350</v>
       </c>
@@ -11455,9 +11443,6 @@
         <v>206</v>
       </c>
       <c r="S41" s="14"/>
-      <c r="T41" s="8" t="s">
-        <v>377</v>
-      </c>
       <c r="U41" s="8" t="s">
         <v>351</v>
       </c>
@@ -11490,9 +11475,6 @@
         <v>230</v>
       </c>
       <c r="S42" s="14"/>
-      <c r="T42" s="8" t="s">
-        <v>375</v>
-      </c>
       <c r="U42" s="8" t="s">
         <v>356</v>
       </c>
@@ -11571,7 +11553,7 @@
         <v>250</v>
       </c>
       <c r="J46" s="14"/>
-      <c r="K46" s="5" t="s">
+      <c r="K46" s="8" t="s">
         <v>563</v>
       </c>
       <c r="L46" s="8" t="s">
@@ -11588,7 +11570,7 @@
       <c r="Q46" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="R46" s="5" t="s">
+      <c r="R46" s="8" t="s">
         <v>567</v>
       </c>
       <c r="S46" s="14"/>
@@ -11624,7 +11606,7 @@
         <v>249</v>
       </c>
       <c r="J47" s="14"/>
-      <c r="K47" s="5" t="s">
+      <c r="K47" s="8" t="s">
         <v>564</v>
       </c>
       <c r="L47" s="8" t="s">
@@ -11641,7 +11623,7 @@
       <c r="Q47" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="R47" s="5" t="s">
+      <c r="R47" s="8" t="s">
         <v>568</v>
       </c>
       <c r="S47" s="14"/>
@@ -11674,7 +11656,7 @@
         <v>248</v>
       </c>
       <c r="J48" s="14"/>
-      <c r="K48" s="5" t="s">
+      <c r="K48" s="8" t="s">
         <v>565</v>
       </c>
       <c r="L48" s="8" t="s">
@@ -11691,7 +11673,7 @@
       <c r="Q48" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="R48" s="5" t="s">
+      <c r="R48" s="8" t="s">
         <v>569</v>
       </c>
       <c r="S48" s="14"/>

</xml_diff>

<commit_message>
Planning update en xml update
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -4522,7 +4522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B346" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B276" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E364" sqref="E364"/>
     </sheetView>
   </sheetViews>
@@ -10458,7 +10458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y89"/>
   <sheetViews>
-    <sheetView topLeftCell="F11" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F11" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>

</xml_diff>